<commit_message>
created the entire menu for the navigation
</commit_message>
<xml_diff>
--- a/MyDatabase.xlsx
+++ b/MyDatabase.xlsx
@@ -17,9 +17,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -72,7 +71,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -89,7 +88,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +355,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="15.71" customWidth="1" style="3" min="1" max="1"/>
     <col width="24.28" customWidth="1" style="3" min="2" max="2"/>
@@ -437,7 +435,7 @@
           <t>Computer Programming</t>
         </is>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="5" t="n">
         <v>45273</v>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -459,15 +457,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="12.14" customWidth="1" style="3" min="6" max="6"/>
+    <col width="14.31" customWidth="1" style="3" min="1" max="2"/>
+    <col width="23.2" customWidth="1" style="3" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="4">
@@ -478,7 +477,7 @@
       </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Section Number</t>
         </is>
       </c>
       <c r="C1" s="3" t="inlineStr">
@@ -502,63 +501,283 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="4">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>MATHF111</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2,</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>M,W,</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="C2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>M,W</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
         <v>5102</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Keskar,Trilok,</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>Trilok,Keskar</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="4">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>MATHF111</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3,4,</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>T,Th,S,</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="C3" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>T,Th,S</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
         <v>5105</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Anirudha,Sharma,</t>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Anirudha,Sharma</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>CSF111</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>6102</v>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Vinti</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="4">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>CSF111</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>2104</v>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Prakhar</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="4">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>CHEMF111</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>M,T,F</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>5105</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>Daksh Jain,Ram Srivastava</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="4">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>CHEMF111</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>T,Th,S</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>5102</v>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Dhyann,Prakhar</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="4">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>CHEMF111</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>6164</v>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>Paritosh</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="4">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>CSF111</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>6168</v>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>Ram</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="4">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>CSF111</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>Th</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>6109</v>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>Abhishek</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MATHF111</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Th</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>6168</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Divyum</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed the way TimeTable.table was created and some more fixes.
</commit_message>
<xml_diff>
--- a/MyDatabase.xlsx
+++ b/MyDatabase.xlsx
@@ -17,8 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -71,7 +72,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -88,6 +89,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,13 +351,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="15.71" customWidth="1" style="3" min="1" max="1"/>
     <col width="24.28" customWidth="1" style="3" min="2" max="2"/>
@@ -439,6 +441,46 @@
         <v>45273</v>
       </c>
       <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>AN</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>BITSF111</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Thermodynamics</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>45271</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>AN</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BITSF112</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Technical Report Writting</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>45269</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>AN</t>
         </is>
@@ -457,13 +499,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="14.31" customWidth="1" style="3" min="1" max="2"/>
     <col width="23.2" customWidth="1" style="3" min="6" max="6"/>
@@ -754,30 +796,58 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>MATHF111</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>T1</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>Th</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="3" t="n">
         <v>6168</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Divyum</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>BITSF112</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Th</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>6164</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Raj</t>
         </is>
       </c>
     </row>

</xml_diff>